<commit_message>
cambio de mapeo transferencia
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -118,10 +118,7 @@
     <t>Productos propios e inscritos Bancolombia</t>
   </si>
   <si>
-    <t>406-732280-07</t>
-  </si>
-  <si>
-    <t>Ahorros</t>
+    <t>406-130790-06</t>
   </si>
   <si>
     <t>userrobot2</t>
@@ -141,10 +138,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -163,6 +160,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -170,14 +174,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +188,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -199,53 +212,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,9 +274,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,30 +283,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,103 +324,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,79 +504,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,11 +533,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,45 +583,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -619,30 +607,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -657,125 +654,125 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1147,7 +1144,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1332,7 +1329,7 @@
         <v>34</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1346,7 +1343,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>22</v>
@@ -1358,7 +1355,7 @@
         <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>26</v>
@@ -1373,7 +1370,7 @@
         <v>29</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N4" t="s">
         <v>31</v>
@@ -1382,7 +1379,7 @@
         <v>100000</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="2">
         <v>40670694007</v>

</xml_diff>

<commit_message>
Modificación en la task de transferencias
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\transferencia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C034CB8-C372-4ADB-9946-EE1DF9E6C599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20130" windowHeight="7425"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -158,19 +164,28 @@
   </si>
   <si>
     <t>RENTA FIJA PLAZO</t>
+  </si>
+  <si>
+    <t>pruebauser01</t>
+  </si>
+  <si>
+    <t>6789</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>406-182800-02</t>
+  </si>
+  <si>
+    <t>406-182800-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,152 +200,8 @@
       <name val="Mic Shell Dlg"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,194 +220,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -559,251 +244,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -821,64 +266,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1165,35 +566,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="11.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="16.8571428571429" customWidth="1"/>
-    <col min="7" max="8" width="15.4285714285714" customWidth="1"/>
-    <col min="9" max="10" width="23.4285714285714" customWidth="1"/>
-    <col min="11" max="11" width="20.7142857142857" customWidth="1"/>
-    <col min="12" max="13" width="16.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="27.8571428571429" customWidth="1"/>
-    <col min="15" max="15" width="12.8571428571429"/>
-    <col min="16" max="16" width="40.2857142857143" customWidth="1"/>
-    <col min="17" max="17" width="22.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875"/>
+    <col min="16" max="16" width="40.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="21" max="21" width="10.5714285714286"/>
-    <col min="22" max="22" width="11.7142857142857"/>
+    <col min="21" max="21" width="10.5703125"/>
+    <col min="22" max="22" width="11.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1312,7 +713,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" customFormat="1" spans="1:19">
+    <row r="3" spans="1:19">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1323,10 +724,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>24</v>
@@ -1350,22 +751,22 @@
         <v>30</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="O3" s="2">
-        <v>100000</v>
+        <v>60000</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="S3" s="2"/>
     </row>
@@ -1483,7 +884,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" customFormat="1" spans="1:19">
+    <row r="6" spans="1:19">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1542,7 +943,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" customFormat="1" spans="1:19">
+    <row r="7" spans="1:19">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1601,7 +1002,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:19">
+    <row r="8" spans="1:19">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1660,12 +1061,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="13:13">
+    <row r="16" spans="1:19">
       <c r="M16" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creación de escenarios para transferencias
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\transferencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C034CB8-C372-4ADB-9946-EE1DF9E6C599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73913D4-A242-4723-8AF0-145B4B424888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -76,9 +76,6 @@
     <t>tipoProductoDestino</t>
   </si>
   <si>
-    <t>opcion</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -124,18 +121,9 @@
     <t>Productos no inscritos Bancolombia</t>
   </si>
   <si>
-    <t>406-739740-05</t>
-  </si>
-  <si>
-    <t>Ahorros</t>
-  </si>
-  <si>
     <t>Productos propios e inscritos Bancolombia</t>
   </si>
   <si>
-    <t>406-739740-07</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -160,12 +148,6 @@
     <t>FIDURENTA</t>
   </si>
   <si>
-    <t>7001000003707</t>
-  </si>
-  <si>
-    <t>RENTA FIJA PLAZO</t>
-  </si>
-  <si>
     <t>pruebauser01</t>
   </si>
   <si>
@@ -179,6 +161,27 @@
   </si>
   <si>
     <t>406-182800-04</t>
+  </si>
+  <si>
+    <t>Mis productos</t>
+  </si>
+  <si>
+    <t>opcionProductoOrigen</t>
+  </si>
+  <si>
+    <t>opcionProductoDestino</t>
+  </si>
+  <si>
+    <t>Inversión</t>
+  </si>
+  <si>
+    <t>0437002003817</t>
+  </si>
+  <si>
+    <t>0009000301809</t>
+  </si>
+  <si>
+    <t>Inscritos</t>
   </si>
 </sst>
 </file>
@@ -248,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -263,11 +266,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -593,11 +597,12 @@
     <col min="16" max="16" width="40.28515625" customWidth="1"/>
     <col min="17" max="17" width="22.140625" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.5703125"/>
     <col min="22" max="22" width="11.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,415 +658,433 @@
         <v>17</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="O2" s="2">
-        <v>100000</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="Q2" s="2">
         <v>40670694007</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="M3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="O3" s="2">
-        <v>60000</v>
+        <v>6000</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="N4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="O4" s="2">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="M5" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O5" s="2">
         <v>100000</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="2">
         <v>40670694007</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="O6" s="2">
         <v>100000</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q6" s="2">
         <v>40670694007</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="M7" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O7" s="2">
         <v>100000</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="S7" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="G8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="M8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="O8" s="2">
-        <v>100000</v>
+        <v>2000</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="M16" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creación de interaction para validar carga de datos y clave dinámica
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\transferencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45A5F09-801E-4258-A609-753941F8E6F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B22A73-11C6-4CEE-91D4-03C9C0F56BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="990" windowWidth="17190" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -139,9 +139,6 @@
     <t>7001000033569</t>
   </si>
   <si>
-    <t>FIDURENTA</t>
-  </si>
-  <si>
     <t>pruebauser01</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>406-182800-02</t>
   </si>
   <si>
-    <t>406-182800-04</t>
-  </si>
-  <si>
     <t>Mis productos</t>
   </si>
   <si>
@@ -179,6 +173,18 @@
   </si>
   <si>
     <t>00004097937784857</t>
+  </si>
+  <si>
+    <t>406-182800-03</t>
+  </si>
+  <si>
+    <t>FIDUCUENTA</t>
+  </si>
+  <si>
+    <t>406-757180-07</t>
+  </si>
+  <si>
+    <t>Ahorros</t>
   </si>
 </sst>
 </file>
@@ -583,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -663,10 +669,10 @@
         <v>17</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -680,10 +686,10 @@
         <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>23</v>
@@ -707,10 +713,10 @@
         <v>29</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O2" s="2">
         <v>1000</v>
@@ -738,10 +744,10 @@
         <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>23</v>
@@ -765,10 +771,10 @@
         <v>29</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="O3" s="2">
         <v>6000</v>
@@ -777,16 +783,16 @@
         <v>33</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -843,10 +849,10 @@
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -918,10 +924,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>23</v>
@@ -945,10 +951,10 @@
         <v>29</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O6" s="2">
         <v>1000</v>
@@ -957,13 +963,13 @@
         <v>36</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="T6" s="2"/>
     </row>
@@ -978,10 +984,10 @@
         <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>23</v>
@@ -1005,28 +1011,28 @@
         <v>29</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="O7" s="2">
-        <v>100000</v>
+        <v>3000</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1040,10 +1046,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>23</v>
@@ -1067,10 +1073,10 @@
         <v>29</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O8" s="2">
         <v>2000</v>
@@ -1079,16 +1085,16 @@
         <v>33</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:20">

</xml_diff>

<commit_message>
Mapeo transferencias a productos no inscritos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\transferencia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/transferencia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B22A73-11C6-4CEE-91D4-03C9C0F56BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="990" windowWidth="17190" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -143,9 +147,6 @@
   </si>
   <si>
     <t>6789</t>
-  </si>
-  <si>
-    <t>Cuenta</t>
   </si>
   <si>
     <t>406-182800-02</t>
@@ -190,8 +191,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,34 +587,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="27.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875"/>
-    <col min="16" max="16" width="40.28515625" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="10" width="23.5" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="27.83203125" customWidth="1"/>
+    <col min="16" max="16" width="40.33203125" customWidth="1"/>
+    <col min="17" max="17" width="22.1640625" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
     <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125"/>
-    <col min="22" max="22" width="11.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,13 +667,13 @@
         <v>17</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -713,10 +711,10 @@
         <v>29</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="O2" s="2">
         <v>1000</v>
@@ -733,7 +731,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -771,7 +769,7 @@
         <v>29</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>31</v>
@@ -783,19 +781,19 @@
         <v>33</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -849,13 +847,13 @@
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -913,7 +911,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -951,10 +949,10 @@
         <v>29</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="O6" s="2">
         <v>1000</v>
@@ -963,17 +961,17 @@
         <v>36</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>31</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1011,10 +1009,10 @@
         <v>29</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O7" s="2">
         <v>3000</v>
@@ -1023,19 +1021,19 @@
         <v>33</v>
       </c>
       <c r="Q7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1073,10 +1071,10 @@
         <v>29</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O8" s="2">
         <v>2000</v>
@@ -1085,19 +1083,19 @@
         <v>33</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="M16" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
División de tipo de transferencias en el datadriven
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/transferencia/Transferencia.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\transferencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8625C8-1E54-4088-9943-FEEE2085EE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A7F05B-9E14-4FF6-8F94-B740367B2E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos" sheetId="1" r:id="rId1"/>
+    <sheet name="MismoBanco" sheetId="5" r:id="rId1"/>
+    <sheet name="OtrosBancos" sheetId="8" r:id="rId2"/>
+    <sheet name="FondosInversion" sheetId="9" r:id="rId3"/>
+    <sheet name="NoInscritos" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -588,11 +591,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A7E926-1581-47D5-9128-BC2D81AC2900}">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -600,6 +603,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="10" width="23.42578125" customWidth="1"/>
@@ -1158,6 +1162,2470 @@
         <v>48</v>
       </c>
     </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="M16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EAF0057-5F47-4619-82E0-8D4003BC3F8B}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="23.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="40.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="2">
+        <v>6000</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3000</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="M16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D6C535-033B-41E5-BE55-7C022CDC74E9}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="40.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="2">
+        <v>6000</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3000</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="M16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0C7D64-2E7C-4E84-8789-69FF86433FA8}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="40.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="2">
+        <v>6000</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3000</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>40670694007</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="16" spans="1:20">
       <c r="M16" s="8"/>
     </row>

</xml_diff>